<commit_message>
Added new files with commands in JSON format
</commit_message>
<xml_diff>
--- a/Reference/Commands.xlsx
+++ b/Reference/Commands.xlsx
@@ -8,15 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="commands" sheetId="1" r:id="rId1"/>
-    <sheet name="git" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="git" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>CMD</t>
   </si>
@@ -84,9 +83,6 @@
     <t>displays the path to the remote origin</t>
   </si>
   <si>
-    <t>git clone http://github.com/jackietrillo/development</t>
-  </si>
-  <si>
     <t>clones a github repository</t>
   </si>
   <si>
@@ -130,6 +126,24 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>git clone url</t>
+  </si>
+  <si>
+    <t>git</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>print working directory</t>
   </si>
 </sst>
 </file>
@@ -461,21 +475,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,19 +503,22 @@
       <c r="D1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -508,63 +526,151 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
-        <v>36</v>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -574,86 +680,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="69.42578125" customWidth="1"/>
     <col min="2" max="2" width="61.42578125" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>